<commit_message>
add a few functions to the original split_into_frag file and rename it all_in_one; the program can now add overhangs to the fragment sequences for gga
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -16,154 +16,154 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
-    <t>CTCCAGCGCGCCTCCTTCTTGGCTTCTCACCTATTCGCACAGTGAAGCCGCCCTCTTGGAAGCTGGCAGGGTCGTTTACCGTCGAACTGACAACATCCGGGTCCTGTGACTCG</t>
-  </si>
-  <si>
-    <t>GCTTCACTTGCGTTTAGATAACAGTGACCGCGGTCATCTTTACTGAGGGCGTTTCCTCCCACAGCTCCTGGCTGGCTTTTCTAGGAGCGAGCAAGGGAAAATTGCCGTTCCTG</t>
-  </si>
-  <si>
-    <t>CGTGGGGCAGATACTTCGTGCTCTCTCGCCGAGCCCGCCTGCGTATCTTGGAAACGCGCGGCGCTTCCTTCCCTACTCCCTTCCGCCTTGGCCGCCCTCATGCTTTAGTCCTG</t>
-  </si>
-  <si>
-    <t>CTCTCGGATTGTATCTGAGCCCTGCCCTTATAGGGTAGCCCCAGGCTTTGCCAATTACTTTCCCATCACTGAATCCAAAAGACAGGAGTTGGGAAAGCCAGCTAATTTCCAGA</t>
-  </si>
-  <si>
-    <t>TGTCATAAATTGAGATTGGAGAAAGGAGCCTAAGTGGGGCTGGGCGGGTCTGAGAGCTCCCGCCAAACCAAAACAAAAAAGAATAGGATGCCAAGGCCGCCGGCATTGGTGGT</t>
-  </si>
-  <si>
-    <t>GCGGAGGGGAGTGTCGGGGTGTGTAGGAGCCACCTCATCCCAGATGGGGGAGTGGAGGTCCTCTGTGGGTGACCCTGACATCCTCCAGGCTTCCCGAACCTACAGAATCACAG</t>
-  </si>
-  <si>
-    <t>ACCCAGGAAGCGCCCTTAGAGATGCCTCACACCCCACTTCCGTCTTGCGTCAGCCTCTTTTCCCTAACGTCTTTCTGACCCTGCTATAGCCCTCCTGGGTAATGGCCAACAGC</t>
-  </si>
-  <si>
-    <t>ACGGAAATGTAGTAGCACCAGGAGTCTGATCACAATTCTGTATGGACAAAGATTCTTCCAGCCTTAGAGGCTAGTTCCTGTTTTCTCCCTCTGCCTCTAAGCCCAACTCCAGC</t>
-  </si>
-  <si>
-    <t>TGGGCCACCCACCCGTAGAGTTTGTACAACTCTCCAACTCTGAGCCTGGAAAGAGGCCTTCCCCAGATATCCCCTAGACAGGATCCCAGGGACACAGCCCACCAGCAGCGCAG</t>
-  </si>
-  <si>
-    <t>CAGGGTGAGGCAGACAGACCAGGAAGCAGAGATGGTGGAATTCTTCACTGCAGAGAAAGAGGGGAAAGCCAGACTTCTGGCCTGGGAATTGACCTAATGGGAACTGTACCAAA</t>
-  </si>
-  <si>
-    <t>GGGTGGGGCCAGATCCTTAGCTGTGGGAACTGACCAGGACCTGGGCTAGACAAGGCAGCTGCCACAGAGCCAGGGCAGAGGTTTGGTCCCTCTGTTGTCCTCATTCCTTGCTC</t>
-  </si>
-  <si>
-    <t>TTTCCCTGGGCCTTCTTTCTATTGTTGAAACACAGCAAATGTGGCCATGGTGGTGGGGGATGGGAAGGACTGCATTTATTTGCCTTGATCCAGCCTGGGAGAAGTCAGGATAG</t>
-  </si>
-  <si>
-    <t>ACTTTGGGCTGCTTGGCCCTGGAGGCAGCTTGAGCTGGGACTGGGGTGGGGGGCTCCTGAGGGGCTGCCTAGGACACTGCAGCTTTTGTGCCTTCTCCCTGCTGCCAACACCC</t>
-  </si>
-  <si>
-    <t>CCACACACACTGCTGCAGCCACTCTAAAGCCCTTTGTCTTTCATTGCTTAGTCACCCCCTTTGTCCTCATCTCAAATAGGGGAGTGGAAAGGGGCAGTAGAGTTCTCTGGTGA</t>
-  </si>
-  <si>
-    <t>TAGCTCCTCTTGCCCCTGCCCCTTCTGGTCTCCCACCCTTTGTCCGACTCCTCTAGTCCCAGCCCCGTTGGCTTAGAACCAGGGTCAGGCAAGTGGTGGGTCAAGAGGTGGGT</t>
-  </si>
-  <si>
-    <t>CTGGCAGTCACAAGGGGGTGGGTGATCCAGGAAGTGATAGGCACCAGGGCAGGTATTACCGACCTGAGCAGGAAGGGAGGGGGAAAGGAAGTATTCTGACGGATATGATATGC</t>
-  </si>
-  <si>
-    <t>GGGGGACAGGAGGTGACAAAGCAGAGTGAATAGGGGAATAGAGGCAAGAGGAGGTGGTCCACTTCTGGGAAAGGAAAGAGACTGCTGACTGCACTCTCCTTCCTGGGGATTTC</t>
-  </si>
-  <si>
-    <t>CTGGGGAAACAAGCAGCCAGAGGATGGGGTGAGCAGAAATTGCCCCTACTTCTGAACCCTTCCTTGCCTTGAGAGTTCATACCCAAGACCTCTTTTCCGAGTTCCCTCCTATC</t>
-  </si>
-  <si>
-    <t>CAAAGCCAAAGGAATAATTTGCTTCCTTTCCCTAACACCACCTCTTCCTCCCCAGCCACTTTCCCCACCCCAGGCAATGGATTTCTCCCAGTACCCTAATTTCCCTATATGCA</t>
-  </si>
-  <si>
-    <t>CAATGCTGTCTCCACCCTCTCCCTGCCCCAGGGAGAATTAAAAAGAAAAGATGACTAGATATTCCAGGAACCACTGGGTTCTCAGAGCAAGGTGGGGTGGATGGTGGGAGCCA</t>
-  </si>
-  <si>
-    <t>GGTGGGGATTCTCCCAGATTGATACTGGGTGAATCTGGGTTCCTGAGAGCAAGTCTTGCCTATGCTGGGGGCTGGCTGACTTGAGGCTGGGGGAGGGTTTAGGGCAGTTGGGA</t>
-  </si>
-  <si>
-    <t>GTGGGTAGGAGCAGGGCCAAAAGCCTGGGGGAAGCTACTGGGAGCTGGGCCAGGGAAATGGGGAGTCAGGAAGTGGGGAGGGGGAACCCTGGGGGGAAATGGAGGCGGAATGG</t>
-  </si>
-  <si>
-    <t>CTGTTCTGGGCTTTGGAGGGGGTGGGTAGTGGTAACTCAGGAAGGGGGATCCTGAGGGAGAGAAGGGACGTTAGAAAAGAGGAGGTGCCACCCTGGATCCGCCTTCTATAAAA</t>
-  </si>
-  <si>
-    <t>GGAAAAGTCGTTAACCCCTCCTGCCTTGTCATCTGCCGCCTCTGTTATGTTCATTCCAAGCAGGATCATCCTACCTTTGGGCAGTCAACTCCCTGATCACTGTCTCCTTGCCT</t>
-  </si>
-  <si>
-    <t>CCCCCAATGTTCTGCCTTTTTTACTCTTCCCAGCTGCTCAGTTCTATCCTGAGCCATGTCAAGCTACCTCTTTTATTTGTTCTTCCCTCTTGATGCCTCCTTACCTGTTCCCT</t>
-  </si>
-  <si>
-    <t>ACCCTCTTTTCTCAGGCAGCTCACTCAGTCCCCTCAGCCCTGGAAACCAGCCACTAGGGCCAAAGGGCAGCATGAGGGAGCCTTGAGAAAAGAGAAGCCATGGTAGGTTAGAC</t>
-  </si>
-  <si>
-    <t>TATAAGAGCAGGAATTCTCCCAGGACCGTGATCCTATCTGTGCATGCCGGCCAGGCCCTTTCCCTCACTCTCTGCCTCTCCTGGGGCTCTGTCCCACCAAAAAGGGAAAGAGA</t>
-  </si>
-  <si>
-    <t>CAGCTGAGGGCTGATTGTGGGGTTTGGGAAAAGGCTATGTCATCAGCTGGCCCAGTGCCTATTATCCATTCGGCTGCTAGAGATTCCCCTCCCCTGGGCAAGTCCCATTTTTT</t>
-  </si>
-  <si>
-    <t>TGGGAAGCGATGATACACCCATCTGAGTCCCACCGACAGAGCTCAGCTGAGTGGCTTAGAGATCAGCCAATCAATCGCAGAGGCTCACCATGCTTAAAAGAGCTGGCGCGGAG</t>
-  </si>
-  <si>
-    <t>AGAGGCTGGGGAGAACCCACAGGGAGACCCACAGACACATATGCACGAGAGAGACAGAGGAGGAAAGAGACAGAGACAAAGGCACAGCGGAAGAAGGCAGAGACAGGGCAGGC</t>
-  </si>
-  <si>
-    <t>ACAGAAGCGGCCCAGACAGAGTCCTACAGAGGGAGAGGCCAGAGAAGCTGCAGAAGACACAGGCAGGGAGAGACAAAGATCCAGGAAAGGAGGGCTCAGGAGGAGAGTTTGGA</t>
-  </si>
-  <si>
-    <t>GAAGCCAGACCCCTGGGCACCTCTCCCAAGCCCAAGGACTAAGTTTTCTCCATTTCCTTTAACGGTCCTCAGCCCTTCTGAAAACTTTGCCTCTGACCTTGGCAGGAGTCCAA</t>
-  </si>
-  <si>
-    <t>GCCCCCAGGCTACAGAGAGGAGCTTTCCAAAGCTAGGGTGTGGAGGACTTGGTGCCCTAGACGGCCTCAGTCCCTCCCAGCTGCAGTACCAGTGCCATGTCCCAGACAGGCTC</t>
-  </si>
-  <si>
-    <t>GCATCCCGGGAGGGGCTTGGCAGGGCGCTGGCTGTGGGGAGCCCAACCCTGCCTCCTGCTCCCCATTGTGCCGCTCTCCTGGCTGGTGTGGCTGCTTCTGCTACTGCTGGCCT</t>
-  </si>
-  <si>
-    <t>CTCTCCTGCCCTCAGCCCGGCTGGCCAGCCCCCTCCCCCGGGAGGAGGAGATCGTGTTTCCAGAGAAGCTCAACGGCAGCGTCCTGCCTGGCTCGGGCGCCCCTGCCAGGCTG</t>
-  </si>
-  <si>
-    <t>TTGTGCCGCTTGCAGGCCTTTGGGGAGACGCTGCTACTAGAGCTGGAGCAGGACTCCGGTGTGCAGGTCGAGGGGCTGACAGTGCAGTACCTGGGCCAGGCGCCTGAGCTGCT</t>
-  </si>
-  <si>
-    <t>GGGTGGAGCAGAGCCTGGCACCTACCTGACTGGCACCATCAATGGAGATCCGGAGTCGGTGGCATCTCTGCACTGGGATGGGGGAGCCCTGTTAGGCGTGTTACAATATCGGG</t>
-  </si>
-  <si>
-    <t>GGGCTGAACTCCACCTCCAGCCCCTGGAGGGAGGCACCCCTAACTCTGCTGGGGGACCTGGGGCTCACATCCTACGCCGGAAGAGTCCTGCCAGCGGTCAAGGTCCCATGTGC</t>
-  </si>
-  <si>
-    <t>AACGTCAAGGCTCCTCTTGGAAGCCCCAGCCCCAGACCCCGAAGAGCCAAGCGCTTTGCTTCACTGAGTAGATTTGTGGAGACACTGGTGGTGGCAGATGACAAGATGGCCGC</t>
-  </si>
-  <si>
-    <t>ATTCCACGGTGCGGGGCTAAAGCGCTACCTGCTAACAGTGATGGCAGCAGCAGCCAAGGCCTTCAAGCACCCAAGCATCCGCAATCCTGTCAGCTTGGTGGTGACTCGGCTAG</t>
-  </si>
-  <si>
-    <t>TGATCCTGGGGTCAGGCGAGGAGGGGCCCCAAGTGGGGCCCAGTGCTGCCCAGACCCTGCGCAGCTTCTGTGCCTGGCAGCGGGGCCTCAACACCCCTGAGGACTCGGACCCT</t>
-  </si>
-  <si>
-    <t>GACCACTTTGACACAGCCATTCTGTTTACCCGTCAGGACCTGTGTGGAGTCTCCACTTGCGACACGCTGGGTATGGCTGATGTGGGCACCGTCTGTGACCCGGCTCGGAGCTG</t>
-  </si>
-  <si>
-    <t>TGCCATTGTGGAGGATGATGGGCTCCAGTCAGCCTTCACTGCTGCTCATGAACTGGGTCATGTCTTCAACATGCTCCATGACAACTCCAAGCCATGCATCAGTTTGAATGGGC</t>
-  </si>
-  <si>
-    <t>CTTTGAGCACCTCTCGCCATGTCATGGCCCCTGTGATGGCTCATGTGGATCCTGAGGAGCCCTGGTCCCCCTGCAGTGCCCGCTTCATCACTGACTTCCTGGACAATGGCTAT</t>
-  </si>
-  <si>
-    <t>GGGCACTGTCTCTTAGACAAACCAGAGGCTCCATTGCATCTGCCTGTGACTTTCCCTGGCAAGGACTATGATGCTGACCGCCAGTGCCAGCTGACCTTCGGGCCCGACTCACG</t>
-  </si>
-  <si>
-    <t>CCATTGTCCACAGCTGCCGCCGCCCTGTGCTGCCCTCTGGTGCTCTGGCCACCTCAATGGCCATGCCATGTGCCAGACCAAACACTCGCCCTGGGCCGATGGCACACCCTGCG</t>
-  </si>
-  <si>
-    <t>GGCCCGCACAGGCCTGCATGGGTGGTCGCTGCCTCCACATGGACCAGCTCCAGGACTTCAATATTCCACAGGCTGGTGGCTGGGGTCCTTGGGGACCATGGGGTGACTGCTCT</t>
-  </si>
-  <si>
-    <t>CGGACCTGTGGGGGTGGTGTCCAGTTCTCCTCCCGAGACTGCACGAGGCCTGTCCCCCGGAATGGTGGCAAGTACTGTGAGGGCCGCCGTACCCGCTTCCGCTCCTGCAACAC</t>
-  </si>
-  <si>
-    <t>TGAGGACTGCCCAACTGGCTCAGGTGGTAGATGGGACCCCCTGTTCCCCGGACAGCTCCTCGGTCTGTGTCCAGGGCCGATGCATCCATGCTGGCTGTGATCGCATCATTGGC</t>
-  </si>
-  <si>
-    <t>TCCAAGAAGAAGTTTGACAAGTGCATGGTGTGCGGAGGGGACGGTTCTGGTTGCAGCAAGCAGTCAGGCTCCTTCAGGAAATTCAGGTACGGATACAACAATGTGGTCACTATCCCCGCGGGG</t>
+    <t>CGTCTCCAGCATTATACAAAGCGGTTCAGGCAGAAAACCCAACAATTCAACATTTTGACGCATCAGTATTTACCGGCGAATACATTACCGGCGCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCGGCGATGTAGATAAAGCTTACCTTGACGCAATTGCACACGCTCGTAATGACAAAGCAAAAGCCAAAGCTGCAAAACAAGCAACCAACGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCCCAATTTAGAAATTCATAACGAAAACTAAATTAAAGCATAAAAACAAGCCCTTGAGTCTGAGATGATTCAAGGGCTTTTTGTATTACGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCATTAATGGCTATATAAAACGATGCCCCTTGAAACCGAAATTTCAAGGGGCAGAGCGTTGCGAGAAATTCATCTCTTATTGTAACAACGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCACAACGTTTTTCATTTCGCAGTGCCATTACAATGATTAAATAGTATCGTTGACATTGATTGTTGTCAATATACATTTATTACAATTCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCAATTTATGATAAAAATTAAACGCCTTGTAAAAAAGGATTATTACAAATTATAAGAGGTGAAATTGTATGAAATTGACGCCATTAAACGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCTAAACTATATTTTAGGTCTTGATTTAGGGATTGCTTCTGTCGGTTGGGCAGTGGTAGAGATTGATGAGCAAGAAAATCCACTAGGTCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCAGGTTTAATTGATGTAGGAGTACGAACATTTGATAGAGCTGAAGTGCCGAAAACAGGCGAAAGTTTGGCATTAGCTCGCCGTTTAGCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCTTAGCTCGTTCTGCTCGTCGTTTAGTAAAACGTCGAGCGGATCGAATTAAAAAAGCGAAGCGTTTATTAAAAGCAGAAAATATTTTCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCTTTTACTTTCGGCAGATGAACACTTGCCCAATGATGTTTGGCAATTACGGGTTAAAGGTTTGGATCAAAAGCTCGAACGCCAGGAACGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCGGAATGGGCAGCGGTTTTATTGCATTTATTGAAACATCGTGGTTATTTGTCACAACGTAAAAATGAAAGCAAAAGTGAGAATAAAGCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCAAAGAATTAGGTGCGTTGCTTTCAGGTGTAGAAACAAACCATCAAATTTTGCAATCTGCTGAATACCGCACGCCTGCGGAAATTGCCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCTTGCTGTGAAGAAATTTCACGTAGAAGATGGGCATATTCGTAATCAGCGTGGTGCTTATACGCATACATTTAGCCGTTTAGATTTACGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCTTTATTGGCGGAAATGGAATTATTGTTCCAACGCCAAACGGACTTGGGCAATCCGCACACTTCTGCAAAATTATTGGAAAATTTGACGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCTTGACCGCTTTATTGATGTGGCAAAAGCCTGCGTTGGCGGGCGAAGCCATTTTGAAAATGCTCGGCAAATGTACCTTTGAACCCACCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCCCACCGAATATAAAGCGGCGAAAAATAGTTATTCGGCTGAGCGTTTTGTATGGCTGACCAAGTTGAATAATTTGCGTATTTTGGAACGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCGGAACAAGGGGCTGAGCGTGCATTGACTGATAACGAACGTTTTGCTCTGCTCGATCAGCCTTATGAAAAAGCCAAGTTTACTTACGCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCTACGCCCAAGCACGTACAATGTTAGCTTTACCTGATGAAGCAATTTTTAAGGGCGTGCGTTATCAAGGCGAAGATAAAAAAGCTGTCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCCTGTCGAAACGAAAACTATTTTAATGGAGATGAAAGCCTATCATCAAATCCGTAAAGCATTAGAGAATGCAGATTTAAAAGCAGAACGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCAGAATGGAATGAACTTAAAAATAATTCCGAATTGCTTGATGACATTGGCACAGCGTTTTCATTGCATAAAACTGATGAAGATATTTCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCATTTGCCGTTATTTAGATGGAAAATTATCGGAAAGCATATTGAATGCGTTGTTAGAAAATCTGAATTTTGACAAATTTATTCAACTCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCAACTTTCACTTAAAGCATTACAACAAATTTTACCGTTGATGTTGCAAGGGCAACGTTATGATGAAGCGGTTTCAGCGATTTATGGTCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCTGGTGATCATTATGGTAAAAAATCAGCAGAAATTAACCGCTTGTTACCAACTATTCCAGCCGATGAAATCCGCAATCCAGTAGTATCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCGTATTACGCACACTGACTCAAGCTCGCAAAGTGATCAATGCGGTGGTGCGATTGTATGGTTCACCTGCTCGTATTCATATTGAAACCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCAAACAGGACGAGAAGTGGGCAAATCTTATCAAGATCGTAAGAAACTGGAGAAACAACAGGAAGATAATCGTAAACAACGTGAAAGTCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCAAGTGCGGTGAAAAAATTCAAAGAATATTTTCCAAATTTCGTGGGAGAGCCAAAAGGTAAAGATATTCTAAAAATGCGTTTGTATGCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCTATGAGTTGCAACAAGCAAAATGTTTATATTCAGGCAAATCATTGGAATTACACCGCTTATTGGAAAAAGGCTATGTAGAAGTTGACGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCTTGATCATGCTTTGCCGTTTTCTCGCACTTGGGATGATAGCTTTAATAATAAAGTGTTGGTGCTTGCCAATGAAAACCAAAATAAACGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCTAAAGGCAATTTAACACCTTATGAATGGTTAGATGGCAAAAATAATAGTGAACATTGGCAAAATTTTGTCGCACGAGTACAAACTACGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCACTAGTGGTTTCTCACATACTAAGAAACAACGTATTTTAAGTCATAAACTAGATGAAAAAGGCTTTATCGAACGTAATTTAAATGACGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCATGATACTCGCTATGTTGCCCGTTTCTTATGTAATTTTATTGCTGACAATATGTTACTGACAGGCAAAGGCAAGCGAAAAGTGTTTCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCGTTTGCTTCAAATGGGCAAATTACGGCTTTATTACGTGGGCGTTGGGGTTTACAAAAAGTACGTGATGATAATGATCGCCACCACGCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCCACGCTTTAGATGCGGTTGTGGTTGCCTGCTCAACGGTAGTGATGCAACAGAAAATTACAAGATTTGTGAGATATGAAGAGGGTAACGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCGTAATGTTTTCAGTGGAGAACGAATTGATCGTGAAACTGGTGAGATTATTCCTTTGCATTTCCCAAGCCCCTGGGCATTTTTTAGACGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCTAGAGAAAATGTGGAAATTCGCATTTTTAGTGAAAATCCGAAATTAGAACTGGAAAATCGCTTACCTGATTATCCACAATATAATCCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCAATCACGAATTTGTTCAGCCGTTATTTGTGTCGAGAATGCCAACCCGAAAAATGACAGGGCAAGGGCATATGGAAACAGTAAAATCCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCAATCAGCCAAACGTTTAGATGAAGGTTTAAGTGTATTAAAAGTGCCTTTAACACAACTTAAATTGAGCGATTTAGAGCGAATGGTTCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCGGTTAATCGTGAGCGTGAAGTTACATTGTACGAATCTTTAAAAGCCCGTTTAGAACAATTTGGTAATGATCCAGCAAAAGCTTTTGCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCTTTGCCGAACCGTTCCATAAAAAAGGCGGTGCGGTGGTTAAAGCTGTGCGAGTGGAACAAACGCAAAAATCAGGCGTATTAGTGCGCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCTGCGTGATGGCAATGGTGTTGCGGATAATGCTTCTATGGTGCGAGTTGATGTCTTTACCAAAGGTGGCAAATACTTCCTTGTGCCACGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCGCCAATTTACACTTGGCAAGTGGCGAAAGGGATTTTGCCAAATAAGGCGGTAACTGCTAATGTTGATGAAATTGATTGGCTTGAAACGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCGAAATGGATGAAAGTTATCAATTTATCTTTACTATGTACCCAAATGATCTTGTCAAAGTAAAATTGAAAAAAGAAGAATTCTTTGGCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCTTGGTTATTACGGTGGTTTAGATCGAGCAACAGGGGCTATTGTCATAAAAGAACACGATTTAGAAAAATCCAAAGGAAAACAAGGTCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCAGGTATTTATCGTATTGGCGTTAAATTAGCTTTGTCATTTGAAAAATACCAAGTCGATGAACTCGGTAAAAATATCCGTCCTTGTCCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCTGTCGTCCAACTAAACGACAACACGTACGCTAACTGAATCCCTACACTCTTCGAGTGTGGGGATTTTTTGTATTTAAGGAAGAAATCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCAAATTATGACTTGGCGTAGTATTTTAATTAGCAAGGGCGGAAAACTTTCCTTGCAGAAAAATCAAATGTTGATTCAGCAAGAGGGTCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCGGGTAATGAATTTACTGTACCTTTGGAAGATATTGCGATTGTAGTGGTGGATAGTCGGGAAACGGTTATTACGATTCCCTTATTATCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCTTATCTGCTTTTGGTTTATACGGCATTACGTTTTTAACTTGTGATGAACAGTTTTTACCTTGTGGGCAATGGTTGCCATTTAATCACGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCATCAATATCATCGACAGCTCAAAACCTTGAAATTACAGCTAGAAGCTAGCTTGCCACAAAAGAAGCAGCTTTGGCAGAAAATTGTGCGAGACG</t>
+  </si>
+  <si>
+    <t>CGTCTCCTGTGCAACAGAAAATCCGAAATCAAGCGACAGTGTTGAAGATTTGCAAATTTCAAGCAGAATCCGACCGCTTGTCTAAAATGGCAGAGCAAGTAAAGAGCACGAGACG</t>
   </si>
 </sst>
 </file>

</xml_diff>